<commit_message>
Office table updated with 2002-11-05 D.A. results
</commit_message>
<xml_diff>
--- a/office_table.xlsx
+++ b/office_table.xlsx
@@ -91,7 +91,7 @@
     <t xml:space="preserve">4 (2, &lt;2008)</t>
   </si>
   <si>
-    <t xml:space="preserve">phase:</t>
+    <t xml:space="preserve">phase (year offset from 2000):</t>
   </si>
   <si>
     <t xml:space="preserve">0, 4</t>
@@ -154,52 +154,52 @@
     <t xml:space="preserve">2002-11-05</t>
   </si>
   <si>
+    <t xml:space="preserve">2003-02-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2003-04-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2003-04-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2003-06-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2003-07-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2003-10-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2003-11-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2004-01-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2004-02-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2004-04-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2004-09-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2004-11-02</t>
+  </si>
+  <si>
     <t xml:space="preserve">pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2003-02-18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2003-04-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2003-04-29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2003-06-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2003-07-22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2003-10-21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2003-11-18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2004-01-27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2004-02-17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2004-04-06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2004-09-14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2004-11-02</t>
   </si>
   <si>
     <t xml:space="preserve">2005-02-15</t>
@@ -465,7 +465,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -476,6 +476,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -502,16 +506,16 @@
   <dimension ref="A1:U98"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.95"/>
@@ -649,9 +653,11 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
       <c r="G3" s="1" t="n">
         <v>0</v>
       </c>
@@ -752,7 +758,7 @@
       <c r="A5" s="1" t="n">
         <v>1849</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -766,7 +772,7 @@
       <c r="A6" s="1" t="n">
         <v>1847</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -777,7 +783,7 @@
       <c r="A7" s="1" t="n">
         <v>1848</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -791,7 +797,7 @@
       <c r="A8" s="1" t="n">
         <v>1846</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -805,7 +811,7 @@
       <c r="A9" s="1" t="n">
         <v>1845</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>36</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -831,7 +837,7 @@
       <c r="A10" s="1" t="n">
         <v>1844</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -845,7 +851,7 @@
       <c r="A11" s="1" t="n">
         <v>1843</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -856,7 +862,7 @@
       <c r="A12" s="1" t="n">
         <v>1842</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -870,7 +876,7 @@
       <c r="A13" s="1" t="n">
         <v>1841</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>41</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -881,7 +887,7 @@
       <c r="A14" s="1" t="n">
         <v>1578</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -916,7 +922,7 @@
       <c r="A15" s="1" t="n">
         <v>1577</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>43</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -941,15 +947,15 @@
         <v>37</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>1840</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>45</v>
+      <c r="B16" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>32</v>
@@ -962,8 +968,8 @@
       <c r="A17" s="1" t="n">
         <v>1839</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>46</v>
+      <c r="B17" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>33</v>
@@ -973,11 +979,11 @@
       <c r="A18" s="1" t="n">
         <v>1756</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>47</v>
+      <c r="B18" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>33</v>
@@ -987,28 +993,28 @@
       <c r="A19" s="1" t="n">
         <v>689</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>685</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>51</v>
+      <c r="B20" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>33</v>
@@ -1018,53 +1024,53 @@
       <c r="A21" s="1" t="n">
         <v>674</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>664</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>54</v>
+      <c r="B22" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>448</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>55</v>
+      <c r="B23" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>447</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>56</v>
+      <c r="B24" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>32</v>
@@ -1077,8 +1083,8 @@
       <c r="A25" s="1" t="n">
         <v>446</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>57</v>
+      <c r="B25" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>33</v>
@@ -1088,8 +1094,8 @@
       <c r="A26" s="1" t="n">
         <v>445</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>58</v>
+      <c r="B26" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>32</v>
@@ -1102,33 +1108,33 @@
       <c r="A27" s="1" t="n">
         <v>444</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="P27" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>443</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1142,7 +1148,7 @@
       <c r="A29" s="1" t="n">
         <v>442</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>61</v>
       </c>
       <c r="O29" s="1" t="s">
@@ -1162,11 +1168,11 @@
       <c r="A30" s="1" t="n">
         <v>441</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>32</v>
@@ -1179,11 +1185,11 @@
       <c r="A31" s="1" t="n">
         <v>440</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q31" s="1" t="s">
         <v>37</v>
@@ -1193,7 +1199,7 @@
       <c r="A32" s="1" t="n">
         <v>439</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>64</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1207,7 +1213,7 @@
       <c r="A33" s="1" t="n">
         <v>438</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>65</v>
       </c>
       <c r="R33" s="1" t="s">
@@ -1224,17 +1230,17 @@
       <c r="A34" s="1" t="n">
         <v>437</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>66</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>37</v>
@@ -1249,23 +1255,23 @@
         <v>37</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="U34" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>436</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="4" t="s">
         <v>67</v>
       </c>
       <c r="H35" s="1" t="s">
@@ -1300,7 +1306,7 @@
       <c r="A36" s="1" t="n">
         <v>435</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1317,7 +1323,7 @@
       <c r="A37" s="1" t="n">
         <v>434</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="4" t="s">
         <v>69</v>
       </c>
       <c r="R37" s="1" t="s">
@@ -1334,7 +1340,7 @@
       <c r="A38" s="1" t="n">
         <v>433</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="4" t="s">
         <v>70</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1348,7 +1354,7 @@
       <c r="A39" s="1" t="n">
         <v>432</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="4" t="s">
         <v>71</v>
       </c>
       <c r="R39" s="1" t="s">
@@ -1365,7 +1371,7 @@
       <c r="A40" s="1" t="n">
         <v>431</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="4" t="s">
         <v>72</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -1385,7 +1391,7 @@
       <c r="A41" s="1" t="n">
         <v>430</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="4" t="s">
         <v>73</v>
       </c>
       <c r="G41" s="1" t="s">
@@ -1408,7 +1414,7 @@
       <c r="A42" s="1" t="n">
         <v>429</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -1425,7 +1431,7 @@
       <c r="A43" s="1" t="n">
         <v>428</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="4" t="s">
         <v>75</v>
       </c>
       <c r="O43" s="1" t="s">
@@ -1445,7 +1451,7 @@
       <c r="A44" s="1" t="n">
         <v>427</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="4" t="s">
         <v>76</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -1462,7 +1468,7 @@
       <c r="A45" s="1" t="n">
         <v>426</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="4" t="s">
         <v>77</v>
       </c>
       <c r="S45" s="1" t="s">
@@ -1476,7 +1482,7 @@
       <c r="A46" s="1" t="n">
         <v>425</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -1514,7 +1520,7 @@
       <c r="A47" s="1" t="n">
         <v>424</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="4" t="s">
         <v>79</v>
       </c>
       <c r="H47" s="1" t="s">
@@ -1546,7 +1552,7 @@
       <c r="A48" s="1" t="n">
         <v>1850</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="4" t="s">
         <v>80</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -1563,7 +1569,7 @@
       <c r="A49" s="1" t="n">
         <v>421</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="4" t="s">
         <v>81</v>
       </c>
       <c r="R49" s="1" t="s">
@@ -1580,11 +1586,11 @@
       <c r="A50" s="1" t="n">
         <v>422</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="4" t="s">
         <v>81</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>32</v>
@@ -1597,11 +1603,11 @@
       <c r="A51" s="1" t="n">
         <v>419</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="4" t="s">
         <v>82</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q51" s="1" t="s">
         <v>37</v>
@@ -1611,11 +1617,11 @@
       <c r="A52" s="1" t="n">
         <v>1837</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>32</v>
@@ -1628,14 +1634,14 @@
       <c r="A53" s="1" t="n">
         <v>1838</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="4" t="s">
         <v>83</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P53" s="1" t="s">
         <v>37</v>
@@ -1645,11 +1651,11 @@
       <c r="A54" s="1" t="n">
         <v>1835</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="4" t="s">
         <v>84</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P54" s="1" t="s">
         <v>37</v>
@@ -1659,14 +1665,14 @@
       <c r="A55" s="1" t="n">
         <v>1836</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="4" t="s">
         <v>84</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P55" s="1" t="s">
         <v>37</v>
@@ -1676,11 +1682,11 @@
       <c r="A56" s="1" t="n">
         <v>1833</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="4" t="s">
         <v>85</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q56" s="1" t="s">
         <v>37</v>
@@ -1690,11 +1696,11 @@
       <c r="A57" s="1" t="n">
         <v>1834</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="4" t="s">
         <v>85</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P57" s="1" t="s">
         <v>37</v>
@@ -1704,11 +1710,11 @@
       <c r="A58" s="1" t="n">
         <v>1832</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="4" t="s">
         <v>86</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P58" s="1" t="s">
         <v>37</v>
@@ -1718,11 +1724,11 @@
       <c r="A59" s="1" t="n">
         <v>416</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="4" t="s">
         <v>87</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>32</v>
@@ -1735,11 +1741,11 @@
       <c r="A60" s="1" t="n">
         <v>415</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="4" t="s">
         <v>88</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q60" s="1" t="s">
         <v>37</v>
@@ -1749,7 +1755,7 @@
       <c r="A61" s="1" t="n">
         <v>1831</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="4" t="s">
         <v>89</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -1763,7 +1769,7 @@
       <c r="A62" s="1" t="n">
         <v>413</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="4" t="s">
         <v>90</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -1783,14 +1789,14 @@
       <c r="A63" s="1" t="n">
         <v>1830</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="4" t="s">
         <v>91</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J63" s="1" t="s">
         <v>37</v>
@@ -1806,11 +1812,11 @@
       <c r="A64" s="1" t="n">
         <v>1662</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>37</v>
@@ -1826,7 +1832,7 @@
       <c r="A65" s="1" t="n">
         <v>411</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -1852,7 +1858,7 @@
       <c r="A66" s="1" t="n">
         <v>409</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="4" t="s">
         <v>94</v>
       </c>
       <c r="G66" s="1" t="s">
@@ -1878,11 +1884,11 @@
       <c r="A67" s="1" t="n">
         <v>410</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="4" t="s">
         <v>94</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>32</v>
@@ -1895,11 +1901,11 @@
       <c r="A68" s="1" t="n">
         <v>408</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="4" t="s">
         <v>95</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P68" s="1" t="s">
         <v>37</v>
@@ -1909,7 +1915,7 @@
       <c r="A69" s="1" t="n">
         <v>1829</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="4" t="s">
         <v>96</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -1926,11 +1932,11 @@
       <c r="A70" s="1" t="n">
         <v>407</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="4" t="s">
         <v>96</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>32</v>
@@ -1943,7 +1949,7 @@
       <c r="A71" s="1" t="n">
         <v>404</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="4" t="s">
         <v>97</v>
       </c>
       <c r="O71" s="1" t="s">
@@ -1963,11 +1969,11 @@
       <c r="A72" s="1" t="n">
         <v>405</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="4" t="s">
         <v>97</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q72" s="1" t="s">
         <v>37</v>
@@ -1977,11 +1983,11 @@
       <c r="A73" s="1" t="n">
         <v>1828</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>32</v>
@@ -1994,11 +2000,11 @@
       <c r="A74" s="1" t="n">
         <v>1827</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="4" t="s">
         <v>99</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q74" s="1" t="s">
         <v>37</v>
@@ -2008,11 +2014,11 @@
       <c r="A75" s="1" t="n">
         <v>1539</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="4" t="s">
         <v>99</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>32</v>
@@ -2025,11 +2031,11 @@
       <c r="A76" s="1" t="n">
         <v>1538</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="4" t="s">
         <v>100</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q76" s="1" t="s">
         <v>37</v>
@@ -2039,7 +2045,7 @@
       <c r="A77" s="1" t="n">
         <v>1826</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="4" t="s">
         <v>101</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -2053,7 +2059,7 @@
       <c r="A78" s="1" t="n">
         <v>1825</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="4" t="s">
         <v>102</v>
       </c>
       <c r="S78" s="1" t="s">
@@ -2067,7 +2073,7 @@
       <c r="A79" s="1" t="n">
         <v>1575</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="4" t="s">
         <v>103</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -2102,7 +2108,7 @@
       <c r="A80" s="1" t="n">
         <v>1574</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="4" t="s">
         <v>104</v>
       </c>
       <c r="I80" s="1" t="s">
@@ -2131,11 +2137,11 @@
       <c r="A81" s="1" t="n">
         <v>1573</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="4" t="s">
         <v>105</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>32</v>
@@ -2151,7 +2157,7 @@
       <c r="A82" s="1" t="n">
         <v>1824</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="4" t="s">
         <v>106</v>
       </c>
       <c r="R82" s="1" t="s">
@@ -2168,11 +2174,11 @@
       <c r="A83" s="1" t="n">
         <v>1576</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" s="4" t="s">
         <v>106</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P83" s="1" t="s">
         <v>37</v>
@@ -2182,11 +2188,11 @@
       <c r="A84" s="1" t="n">
         <v>1661</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B84" s="4" t="s">
         <v>107</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>32</v>
@@ -2199,11 +2205,11 @@
       <c r="A85" s="1" t="n">
         <v>1660</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="4" t="s">
         <v>108</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P85" s="1" t="s">
         <v>37</v>
@@ -2213,11 +2219,11 @@
       <c r="A86" s="1" t="n">
         <v>1659</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B86" s="4" t="s">
         <v>109</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>32</v>
@@ -2230,11 +2236,11 @@
       <c r="A87" s="1" t="n">
         <v>1658</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="4" t="s">
         <v>110</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q87" s="1" t="s">
         <v>37</v>
@@ -2244,7 +2250,7 @@
       <c r="A88" s="1" t="n">
         <v>1823</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="4" t="s">
         <v>111</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -2261,7 +2267,7 @@
       <c r="A89" s="1" t="n">
         <v>1865</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="4" t="s">
         <v>112</v>
       </c>
       <c r="R89" s="1" t="s">
@@ -2278,7 +2284,7 @@
       <c r="A90" s="1" t="n">
         <v>1710</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="4" t="s">
         <v>112</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -2292,7 +2298,7 @@
       <c r="A91" s="1" t="n">
         <v>1711</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="4" t="s">
         <v>113</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -2318,7 +2324,7 @@
       <c r="A92" s="1" t="n">
         <v>1748</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B92" s="4" t="s">
         <v>114</v>
       </c>
       <c r="G92" s="1" t="s">
@@ -2341,7 +2347,7 @@
       <c r="A93" s="1" t="n">
         <v>1755</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B93" s="4" t="s">
         <v>115</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -2358,7 +2364,7 @@
       <c r="A94" s="1" t="n">
         <v>1761</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B94" s="4" t="s">
         <v>116</v>
       </c>
       <c r="O94" s="1" t="s">
@@ -2378,11 +2384,11 @@
       <c r="A95" s="1" t="n">
         <v>1822</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B95" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>32</v>
@@ -2398,11 +2404,11 @@
       <c r="A96" s="1" t="n">
         <v>1851</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B96" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P96" s="1" t="s">
         <v>37</v>
@@ -2415,7 +2421,7 @@
       <c r="A97" s="1" t="n">
         <v>1864</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B97" s="4" t="s">
         <v>119</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -2432,7 +2438,7 @@
       <c r="A98" s="1" t="n">
         <v>1866</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B98" s="4" t="s">
         <v>120</v>
       </c>
       <c r="R98" s="1" t="s">
@@ -2446,6 +2452,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:C3"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Add 2018-05-15 and 2018-06-12 elections with tests
</commit_message>
<xml_diff>
--- a/office_table.xlsx
+++ b/office_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="123">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -383,6 +383,12 @@
   </si>
   <si>
     <t xml:space="preserve">2018-04-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-05-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-12</t>
   </si>
 </sst>
 </file>
@@ -478,7 +484,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -503,12 +509,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U98"/>
+  <dimension ref="A1:U100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="4" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
+      <selection pane="bottomLeft" activeCell="A100" activeCellId="0" sqref="100:100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2451,6 +2457,43 @@
         <v>37</v>
       </c>
     </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="n">
+        <v>1873</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P99" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q99" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="n">
+        <v>1874</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P100" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q100" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A3:C3"/>

</xml_diff>

<commit_message>
Added Presidential primary results to 2008-02-19 election (id 433)
</commit_message>
<xml_diff>
--- a/office_table.xlsx
+++ b/office_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="124">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t xml:space="preserve">2012-04-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P/-/-</t>
   </si>
   <si>
     <t xml:space="preserve">2012-05-08</t>
@@ -512,9 +515,9 @@
   <dimension ref="A1:U100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A100" activeCellId="0" sqref="100:100"/>
+      <selection pane="bottomLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1352,6 +1355,9 @@
       <c r="D38" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G38" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="T38" s="1" t="s">
         <v>37</v>
       </c>
@@ -1779,7 +1785,7 @@
         <v>90</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>37</v>
@@ -1796,7 +1802,7 @@
         <v>1830</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>32</v>
@@ -1819,7 +1825,7 @@
         <v>1662</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>52</v>
@@ -1839,7 +1845,7 @@
         <v>411</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>32</v>
@@ -1865,7 +1871,7 @@
         <v>409</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>37</v>
@@ -1891,7 +1897,7 @@
         <v>410</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>47</v>
@@ -1908,7 +1914,7 @@
         <v>408</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>47</v>
@@ -1922,7 +1928,7 @@
         <v>1829</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>32</v>
@@ -1939,7 +1945,7 @@
         <v>407</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>47</v>
@@ -1956,7 +1962,7 @@
         <v>404</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O71" s="1" t="s">
         <v>37</v>
@@ -1976,7 +1982,7 @@
         <v>405</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>47</v>
@@ -1990,7 +1996,7 @@
         <v>1828</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>47</v>
@@ -2007,7 +2013,7 @@
         <v>1827</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>47</v>
@@ -2021,7 +2027,7 @@
         <v>1539</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>47</v>
@@ -2038,7 +2044,7 @@
         <v>1538</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>47</v>
@@ -2052,7 +2058,7 @@
         <v>1826</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>32</v>
@@ -2066,7 +2072,7 @@
         <v>1825</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="S78" s="1" t="s">
         <v>37</v>
@@ -2080,7 +2086,7 @@
         <v>1575</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>32</v>
@@ -2115,7 +2121,7 @@
         <v>1574</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>37</v>
@@ -2144,7 +2150,7 @@
         <v>1573</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>47</v>
@@ -2164,7 +2170,7 @@
         <v>1824</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="R82" s="1" t="s">
         <v>37</v>
@@ -2181,7 +2187,7 @@
         <v>1576</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>47</v>
@@ -2195,7 +2201,7 @@
         <v>1661</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>47</v>
@@ -2212,7 +2218,7 @@
         <v>1660</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>47</v>
@@ -2226,7 +2232,7 @@
         <v>1659</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>47</v>
@@ -2243,7 +2249,7 @@
         <v>1658</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>47</v>
@@ -2257,7 +2263,7 @@
         <v>1823</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>32</v>
@@ -2274,7 +2280,7 @@
         <v>1865</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="R89" s="1" t="s">
         <v>37</v>
@@ -2291,7 +2297,7 @@
         <v>1710</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>32</v>
@@ -2305,7 +2311,7 @@
         <v>1711</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>32</v>
@@ -2331,7 +2337,7 @@
         <v>1748</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>37</v>
@@ -2354,7 +2360,7 @@
         <v>1755</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>32</v>
@@ -2371,7 +2377,7 @@
         <v>1761</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="O94" s="1" t="s">
         <v>37</v>
@@ -2391,7 +2397,7 @@
         <v>1822</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>47</v>
@@ -2411,7 +2417,7 @@
         <v>1851</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>47</v>
@@ -2428,7 +2434,7 @@
         <v>1864</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>32</v>
@@ -2445,7 +2451,7 @@
         <v>1866</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="R98" s="1" t="s">
         <v>37</v>
@@ -2462,7 +2468,7 @@
         <v>1873</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>47</v>
@@ -2482,7 +2488,7 @@
         <v>1874</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Add 2018-11-06 election metadata, input files, results, tests, & update office_table
</commit_message>
<xml_diff>
--- a/office_table.xlsx
+++ b/office_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="125">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -392,6 +392,9 @@
   </si>
   <si>
     <t xml:space="preserve">2018-06-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-11-06</t>
   </si>
 </sst>
 </file>
@@ -512,12 +515,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U100"/>
+  <dimension ref="A1:U102"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
+      <selection pane="bottomLeft" activeCell="A104" activeCellId="0" sqref="104:104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2500,6 +2503,38 @@
         <v>37</v>
       </c>
     </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="n">
+        <v>1886</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J102" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L102" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M102" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N102" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P102" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q102" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A3:C3"/>

</xml_diff>

<commit_message>
Add 2018-08-14 election to office_table.xlsx
</commit_message>
<xml_diff>
--- a/office_table.xlsx
+++ b/office_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="126">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -392,6 +392,12 @@
   </si>
   <si>
     <t xml:space="preserve">2018-06-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-11-06</t>
   </si>
 </sst>
 </file>
@@ -512,12 +518,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U100"/>
+  <dimension ref="A1:U102"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
+      <selection pane="bottomLeft" activeCell="B105" activeCellId="0" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2500,6 +2506,76 @@
         <v>37</v>
       </c>
     </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="n">
+        <v>1878</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K101" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L101" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M101" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N101" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P101" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q101" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="n">
+        <v>1886</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J102" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L102" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M102" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N102" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P102" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q102" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A3:C3"/>

</xml_diff>